<commit_message>
Atualizações nas documentações: modelo UML e Product Backlog Finalização da tela de cadastro do cliente e avanços na JanelaPrincipal Criação de ClienteDao gravando no banco de dados Adicionado no arquico de SQL o comando de criação da tabela tbCliente
</commit_message>
<xml_diff>
--- a/Locadora de Veiculos/Documentacao do Projeto/Product Backlog Locadora de Veiculos.xlsx
+++ b/Locadora de Veiculos/Documentacao do Projeto/Product Backlog Locadora de Veiculos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
   <si>
     <t>Item</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>Data realização</t>
+  </si>
+  <si>
+    <t>Feito</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -200,8 +206,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="h:mm;@"/>
-    <numFmt numFmtId="168" formatCode="[$-416]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="[$-416]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -509,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,15 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -585,26 +582,96 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -617,57 +684,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1015,10 +1031,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="50"/>
       <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1042,7 +1058,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="27">
+      <c r="A4" s="51">
         <v>3</v>
       </c>
       <c r="B4" s="6"/>
@@ -1051,7 +1067,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
@@ -1060,7 +1076,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
@@ -1069,7 +1085,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1078,7 +1094,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="27">
+      <c r="A8" s="51">
         <v>4</v>
       </c>
       <c r="B8" s="6"/>
@@ -1087,7 +1103,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
@@ -1096,7 +1112,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
@@ -1105,7 +1121,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
@@ -1114,7 +1130,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="8" t="s">
         <v>18</v>
       </c>
@@ -1123,7 +1139,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="8" t="s">
         <v>19</v>
       </c>
@@ -1150,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,9 +1176,9 @@
     <col min="2" max="2" width="8.85546875" style="17" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="39"/>
+    <col min="5" max="5" width="9.140625" style="36"/>
     <col min="6" max="6" width="9.140625" style="17"/>
-    <col min="7" max="7" width="14.42578125" style="60" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="44" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
@@ -1179,26 +1195,26 @@
       <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="30" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="38" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="47"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="54"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
@@ -1211,13 +1227,13 @@
       <c r="D3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="34">
+      <c r="E3" s="31">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="55">
+      <c r="G3" s="39">
         <v>42503</v>
       </c>
     </row>
@@ -1232,13 +1248,13 @@
       <c r="D4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="32">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="F4" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="56">
+      <c r="G4" s="40">
         <v>42503</v>
       </c>
     </row>
@@ -1253,13 +1269,15 @@
       <c r="D5" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="32">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="56"/>
+      <c r="G5" s="40">
+        <v>42506</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
@@ -1272,13 +1290,15 @@
       <c r="D6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="32">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="F6" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="56"/>
+      <c r="G6" s="40">
+        <v>42506</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
@@ -1291,13 +1311,15 @@
       <c r="D7" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="32">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="56"/>
+      <c r="G7" s="40">
+        <v>42506</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
@@ -1310,13 +1332,15 @@
       <c r="D8" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="56"/>
+      <c r="G8" s="40">
+        <v>42513</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
@@ -1329,13 +1353,15 @@
       <c r="D9" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="32">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="56"/>
+      <c r="G9" s="40">
+        <v>42506</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
@@ -1348,13 +1374,15 @@
       <c r="D10" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F10" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="56"/>
+      <c r="G10" s="40">
+        <v>42506</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
@@ -1367,13 +1395,15 @@
       <c r="D11" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="32">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="F11" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="56"/>
+      <c r="G11" s="40">
+        <v>42506</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
@@ -1386,13 +1416,13 @@
       <c r="D12" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F12" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="56"/>
+      <c r="G12" s="40"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
@@ -1405,13 +1435,13 @@
       <c r="D13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="56"/>
+      <c r="G13" s="40"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
@@ -1424,13 +1454,15 @@
       <c r="D14" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="32">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="F14" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="56"/>
+      <c r="G14" s="40">
+        <v>42506</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
@@ -1443,13 +1475,13 @@
       <c r="D15" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="56"/>
+      <c r="G15" s="40"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
@@ -1462,13 +1494,13 @@
       <c r="D16" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="35">
+      <c r="E16" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F16" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="56"/>
+      <c r="G16" s="40"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
@@ -1481,47 +1513,47 @@
       <c r="D17" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="32">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F17" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="56"/>
+      <c r="G17" s="40"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
       <c r="B18" s="24"/>
       <c r="C18" s="24"/>
       <c r="D18" s="23"/>
-      <c r="E18" s="36"/>
+      <c r="E18" s="33"/>
       <c r="F18" s="24"/>
-      <c r="G18" s="57"/>
+      <c r="G18" s="41"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="29"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="29" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="37">
+      <c r="E19" s="34">
         <f>SUM(E3:E17)</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="F19" s="30"/>
-      <c r="G19" s="58"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="42"/>
     </row>
     <row r="20" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="57"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
@@ -1534,13 +1566,13 @@
       <c r="D21" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="34">
+      <c r="E21" s="31">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F21" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G21" s="55"/>
+      <c r="G21" s="39"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
@@ -1553,13 +1585,13 @@
       <c r="D22" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="35">
+      <c r="E22" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F22" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G22" s="56"/>
+      <c r="G22" s="40"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
@@ -1569,41 +1601,43 @@
       <c r="C23" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="36">
+      <c r="E23" s="33">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="F23" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G23" s="57"/>
+      <c r="G23" s="40">
+        <v>42506</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="29"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="29" t="s">
+      <c r="A24" s="26"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="37">
+      <c r="E24" s="34">
         <f>SUM(E21:E23)</f>
         <v>9.722222222222221E-2</v>
       </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="58"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="42"/>
     </row>
     <row r="25" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="53"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="60"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
@@ -1616,117 +1650,117 @@
       <c r="D26" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="34">
+      <c r="E26" s="31">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="F26" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="55"/>
+      <c r="G26" s="39"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="19"/>
-      <c r="E27" s="35"/>
+      <c r="E27" s="32"/>
       <c r="F27" s="20"/>
-      <c r="G27" s="56"/>
+      <c r="G27" s="40"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="29" t="s">
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="38">
+      <c r="E28" s="35">
         <f>SUM(E26:E27)</f>
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="F28" s="32"/>
-      <c r="G28" s="59"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="43"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="19"/>
-      <c r="E29" s="35"/>
+      <c r="E29" s="32"/>
       <c r="F29" s="20"/>
-      <c r="G29" s="56"/>
+      <c r="G29" s="40"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="19"/>
-      <c r="E30" s="35"/>
+      <c r="E30" s="32"/>
       <c r="F30" s="20"/>
-      <c r="G30" s="56"/>
+      <c r="G30" s="40"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="19"/>
-      <c r="E31" s="35"/>
+      <c r="E31" s="32"/>
       <c r="F31" s="20"/>
-      <c r="G31" s="56"/>
+      <c r="G31" s="40"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
       <c r="D32" s="19"/>
-      <c r="E32" s="35"/>
+      <c r="E32" s="32"/>
       <c r="F32" s="20"/>
-      <c r="G32" s="56"/>
+      <c r="G32" s="40"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
       <c r="D33" s="19"/>
-      <c r="E33" s="35"/>
+      <c r="E33" s="32"/>
       <c r="F33" s="20"/>
-      <c r="G33" s="56"/>
+      <c r="G33" s="40"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
       <c r="D34" s="19"/>
-      <c r="E34" s="35"/>
+      <c r="E34" s="32"/>
       <c r="F34" s="20"/>
-      <c r="G34" s="56"/>
+      <c r="G34" s="40"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
       <c r="D35" s="19"/>
-      <c r="E35" s="35"/>
+      <c r="E35" s="32"/>
       <c r="F35" s="20"/>
-      <c r="G35" s="56"/>
+      <c r="G35" s="40"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="19"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
       <c r="D36" s="19"/>
-      <c r="E36" s="35"/>
+      <c r="E36" s="32"/>
       <c r="F36" s="20"/>
-      <c r="G36" s="56"/>
+      <c r="G36" s="40"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
       <c r="D37" s="19"/>
-      <c r="E37" s="35"/>
+      <c r="E37" s="32"/>
       <c r="F37" s="20"/>
-      <c r="G37" s="56"/>
+      <c r="G37" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1741,28 +1775,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="44"/>
+    <col min="4" max="5" width="9.140625" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -1772,11 +1812,14 @@
       <c r="C2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="31">
         <v>6.9444444444444441E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -1786,11 +1829,14 @@
       <c r="C3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="32">
         <v>1.3888888888888888E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -1800,11 +1846,14 @@
       <c r="C4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="32">
         <v>3.472222222222222E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -1814,11 +1863,14 @@
       <c r="C5" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="32">
         <v>3.472222222222222E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <v>7</v>
       </c>
@@ -1828,11 +1880,14 @@
       <c r="C6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="32">
         <v>2.0833333333333332E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="22">
         <v>5</v>
       </c>
@@ -1842,11 +1897,14 @@
       <c r="C7" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="32">
         <v>6.9444444444444441E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="22">
         <v>6</v>
       </c>
@@ -1856,11 +1914,14 @@
       <c r="C8" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
         <v>8</v>
       </c>
@@ -1870,25 +1931,31 @@
       <c r="C9" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10" s="38">
+      <c r="E9" s="47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="35">
         <f>SUM(D2:D9)</f>
         <v>0.13888888888888887</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="42" t="s">
+    <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="22">
         <v>9</v>
       </c>
@@ -1898,11 +1965,14 @@
       <c r="C13" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="32">
         <v>1.3888888888888888E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="22">
         <v>10</v>
       </c>
@@ -1912,11 +1982,12 @@
       <c r="C14" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="47"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="22">
         <v>11</v>
       </c>
@@ -1926,11 +1997,12 @@
       <c r="C15" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="47"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>18</v>
       </c>
@@ -1940,25 +2012,35 @@
       <c r="C16" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="32">
         <v>1.3888888888888888E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="38">
+      <c r="E16" s="47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="35">
         <f>SUM(D13:D16)</f>
         <v>0.1111111111111111</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="42" t="s">
+      <c r="E17" s="48"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="48"/>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="64"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
         <v>12</v>
       </c>
@@ -1968,11 +2050,14 @@
       <c r="C20" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="35">
+      <c r="D20" s="32">
         <v>1.3888888888888888E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="22">
         <v>13</v>
       </c>
@@ -1982,11 +2067,12 @@
       <c r="C21" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D21" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="47"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="22">
         <v>14</v>
       </c>
@@ -1996,11 +2082,12 @@
       <c r="C22" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="35">
+      <c r="D22" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="47"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="22">
         <v>16</v>
       </c>
@@ -2010,25 +2097,29 @@
       <c r="C23" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="34">
+      <c r="D23" s="31">
         <v>4.1666666666666664E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="38">
+      <c r="E23" s="47"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="35">
         <f>SUM(D20:D23)</f>
         <v>0.13888888888888887</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="42" t="s">
+    <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="22">
         <v>15</v>
       </c>
@@ -2038,11 +2129,12 @@
       <c r="C27" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="35">
+      <c r="D27" s="32">
         <v>8.3333333333333329E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="47"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>17</v>
       </c>
@@ -2052,11 +2144,12 @@
       <c r="C28" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="35">
+      <c r="D28" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="47"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="22">
         <v>19</v>
       </c>
@@ -2066,12 +2159,13 @@
       <c r="C29" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="34">
+      <c r="D29" s="31">
         <v>3.472222222222222E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D30" s="38">
+      <c r="E29" s="47"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="35">
         <f>SUM(D27:D29)</f>
         <v>0.12847222222222221</v>
       </c>

</xml_diff>

<commit_message>
Funcionando: Cadastro de Clientes, Cadastro de Veículos e Pesquisa de Cliente por CNH. Documentação do projeto atualizada.
</commit_message>
<xml_diff>
--- a/Locadora de Veiculos/Documentacao do Projeto/Product Backlog Locadora de Veiculos.xlsx
+++ b/Locadora de Veiculos/Documentacao do Projeto/Product Backlog Locadora de Veiculos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="61">
   <si>
     <t>Item</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Desenvolver o relatório aluguéis realizados</t>
   </si>
   <si>
-    <t>Criar relatório de clientes cadastrados</t>
-  </si>
-  <si>
     <t>Criar relatório de veículos cadastrados</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Alterado - Criar pesquisa de cliente por CNH</t>
   </si>
 </sst>
 </file>
@@ -1166,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,7 +1202,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -1231,7 +1231,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3" s="39">
         <v>42503</v>
@@ -1252,7 +1252,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G4" s="40">
         <v>42503</v>
@@ -1273,7 +1273,7 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5" s="40">
         <v>42506</v>
@@ -1294,7 +1294,7 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G6" s="40">
         <v>42506</v>
@@ -1315,7 +1315,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G7" s="40">
         <v>42506</v>
@@ -1336,7 +1336,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8" s="40">
         <v>42513</v>
@@ -1357,7 +1357,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9" s="40">
         <v>42506</v>
@@ -1372,13 +1372,13 @@
         <v>10</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G10" s="40">
         <v>42506</v>
@@ -1399,7 +1399,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11" s="40">
         <v>42506</v>
@@ -1420,9 +1420,11 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="40"/>
+        <v>56</v>
+      </c>
+      <c r="G12" s="40">
+        <v>42517</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
@@ -1439,9 +1441,11 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="40"/>
+        <v>56</v>
+      </c>
+      <c r="G13" s="40">
+        <v>42516</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
@@ -1449,7 +1453,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>40</v>
@@ -1458,7 +1462,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G14" s="40">
         <v>42506</v>
@@ -1470,7 +1474,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>41</v>
@@ -1479,7 +1483,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G15" s="40"/>
     </row>
@@ -1489,7 +1493,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>43</v>
@@ -1498,7 +1502,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G16" s="40"/>
     </row>
@@ -1517,7 +1521,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G17" s="40"/>
     </row>
@@ -1535,7 +1539,7 @@
       <c r="B19" s="27"/>
       <c r="C19" s="27"/>
       <c r="D19" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="34">
         <f>SUM(E3:E17)</f>
@@ -1564,15 +1568,17 @@
         <v>15</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="E21" s="31">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="39"/>
+        <v>56</v>
+      </c>
+      <c r="G21" s="39">
+        <v>42517</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
@@ -1583,13 +1589,13 @@
         <v>16</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G22" s="40"/>
     </row>
@@ -1602,13 +1608,13 @@
         <v>22</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E23" s="33">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G23" s="40">
         <v>42506</v>
@@ -1619,7 +1625,7 @@
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
       <c r="D24" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="34">
         <f>SUM(E21:E23)</f>
@@ -1648,13 +1654,13 @@
         <v>22</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="31">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G26" s="39"/>
     </row>
@@ -1672,7 +1678,7 @@
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
       <c r="D28" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E28" s="35">
         <f>SUM(E26:E27)</f>
@@ -1777,8 +1783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,13 +1796,13 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="61" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
       <c r="D1" s="62"/>
       <c r="E1" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1" s="45"/>
       <c r="G1" s="45"/>
@@ -1816,7 +1822,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E2" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1833,7 +1839,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1850,7 +1856,7 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1867,7 +1873,7 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1884,7 +1890,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E6" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1901,7 +1907,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1918,7 +1924,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E8" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1929,13 +1935,13 @@
         <v>10</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E9" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1946,13 +1952,13 @@
     </row>
     <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="64"/>
       <c r="C12" s="64"/>
       <c r="D12" s="64"/>
       <c r="E12" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1969,7 +1975,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="E13" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1985,7 +1991,9 @@
       <c r="D14" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E14" s="47"/>
+      <c r="E14" s="47" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="22">
@@ -2000,7 +2008,9 @@
       <c r="D15" s="32">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E15" s="47"/>
+      <c r="E15" s="47" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
@@ -2010,13 +2020,13 @@
         <v>22</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" s="32">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="E16" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2031,13 +2041,13 @@
     </row>
     <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="64"/>
       <c r="C19" s="64"/>
       <c r="D19" s="64"/>
       <c r="E19" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2045,7 +2055,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>40</v>
@@ -2054,7 +2064,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="E20" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2062,7 +2072,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>41</v>
@@ -2077,7 +2087,7 @@
         <v>14</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>43</v>
@@ -2095,12 +2105,14 @@
         <v>15</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D23" s="31">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E23" s="47"/>
+      <c r="E23" s="47" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D24" s="35">
@@ -2110,13 +2122,13 @@
     </row>
     <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="64"/>
       <c r="C26" s="64"/>
       <c r="D26" s="64"/>
       <c r="E26" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2142,7 +2154,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" s="32">
         <v>4.1666666666666664E-2</v>
@@ -2157,7 +2169,7 @@
         <v>22</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="31">
         <v>3.472222222222222E-3</v>

</xml_diff>